<commit_message>
With Models changes done with Fer
</commit_message>
<xml_diff>
--- a/books-apis-baseline.xlsx
+++ b/books-apis-baseline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorge_guzman/bootCampClasses/projects/project2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5DF15C6-195F-B848-B38B-9D1C01D25E5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4558B8-2D0A-C142-BFDD-693BDA52FD82}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="36600" windowHeight="22660" activeTab="1" xr2:uid="{86F54AEE-F7BE-1B46-B9C2-50DD7E0F702B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="31400" windowHeight="22660" activeTab="1" xr2:uid="{86F54AEE-F7BE-1B46-B9C2-50DD7E0F702B}"/>
   </bookViews>
   <sheets>
     <sheet name="api" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="164">
   <si>
     <t>Sign up / Log in</t>
   </si>
@@ -113,9 +113,6 @@
   </si>
   <si>
     <t>"/api/books"</t>
-  </si>
-  <si>
-    <t>"/api/category/:id"</t>
   </si>
   <si>
     <t>Click on a category</t>
@@ -536,9 +533,6 @@
     <t>purchases_books</t>
   </si>
   <si>
-    <t>purchase_id</t>
-  </si>
-  <si>
     <t>how to normalize databases</t>
   </si>
   <si>
@@ -582,6 +576,77 @@
   </si>
   <si>
     <t>DATETIME</t>
+  </si>
+  <si>
+    <t>categories</t>
+  </si>
+  <si>
+    <t>thumbnail</t>
+  </si>
+  <si>
+    <t>subtitle</t>
+  </si>
+  <si>
+    <t>TEXT</t>
+  </si>
+  <si>
+    <t>published_year</t>
+  </si>
+  <si>
+    <t>average_rating</t>
+  </si>
+  <si>
+    <t>num_pages</t>
+  </si>
+  <si>
+    <t>DECIMA (10,0)</t>
+  </si>
+  <si>
+    <t>INT (FK ??)</t>
+  </si>
+  <si>
+    <t>INT PK (FK ??)</t>
+  </si>
+  <si>
+    <t>Click on a book</t>
+  </si>
+  <si>
+    <t>Select a category and display 10 books</t>
+  </si>
+  <si>
+    <t>[
+{
+   id: xxx,
+   title: xxx,
+   authors, xxx,
+   category: xxx,
+   thumbnail_url: xxx,
+   description: xxx,
+   year: xxx,
+   rating: xxx,
+   pages: xxx,
+   ratings_count: xxx,
+   price: xxx
+}
+]</t>
+  </si>
+  <si>
+    <t>"/api/books/:id"</t>
+  </si>
+  <si>
+    <t>"/api/books/category/:id"</t>
+  </si>
+  <si>
+    <t>UserId</t>
+  </si>
+  <si>
+    <t>BookId</t>
+  </si>
+  <si>
+    <t>PurchaseId</t>
+  </si>
+  <si>
+    <t>ShoppingcartId</t>
   </si>
 </sst>
 </file>
@@ -662,7 +727,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,6 +758,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -706,7 +777,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -773,12 +844,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -787,11 +852,41 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1637,13 +1732,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E085F2A6-2F83-794C-A2D7-43C9D476331B}">
-  <dimension ref="B1:R28"/>
+  <dimension ref="B1:R29"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J11" sqref="J11"/>
+      <selection pane="bottomRight" activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1674,22 +1769,22 @@
     <row r="1" spans="2:18" ht="8" customHeight="1"/>
     <row r="2" spans="2:18">
       <c r="B2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>117</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>3</v>
@@ -1698,16 +1793,16 @@
         <v>4</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="L2" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M2" s="22"/>
       <c r="N2" s="22"/>
       <c r="O2"/>
       <c r="P2" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="Q2" s="22"/>
       <c r="R2" s="22"/>
@@ -1717,338 +1812,338 @@
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L3" s="17" t="s">
         <v>4</v>
       </c>
       <c r="M3" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="N3" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="O3"/>
       <c r="P3" s="17" t="s">
         <v>4</v>
       </c>
       <c r="Q3" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="R3" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="17" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="4" spans="2:18">
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H4" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J4" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>62</v>
-      </c>
       <c r="L4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N4" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="16" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="Q4" s="16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="R4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="2:18">
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>63</v>
+      <c r="G5" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I5" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>62</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="N5" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O5" s="18"/>
       <c r="P5" s="16"/>
       <c r="Q5" s="19" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="R5" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18">
+      <c r="C6" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="M6" s="16" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="6" spans="2:18">
-      <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I6" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>77</v>
-      </c>
       <c r="N6" s="16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O6" s="18"/>
       <c r="P6" s="16"/>
       <c r="Q6" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" spans="2:18">
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>65</v>
+      <c r="G7" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I7" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>64</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O7" s="18"/>
       <c r="P7" s="16"/>
       <c r="Q7" s="19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" spans="2:18">
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>66</v>
+      <c r="G8" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I8" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="M8" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="N8" s="21" t="s">
         <v>92</v>
-      </c>
-      <c r="N8" s="21" t="s">
-        <v>93</v>
       </c>
       <c r="O8" s="18"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="2:18">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>67</v>
+      <c r="G9" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>66</v>
       </c>
       <c r="M9" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="N9" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O9"/>
       <c r="Q9" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="R9" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="R9" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="187">
       <c r="B10" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C10" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I10" s="2" t="s">
+      <c r="G10" s="39" t="s">
+        <v>93</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="J10" s="11" t="s">
-        <v>110</v>
+      <c r="I10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>109</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O10"/>
       <c r="Q10" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="2:18" ht="187">
       <c r="C11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>23</v>
@@ -2060,558 +2155,584 @@
         <v>22</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="M11" s="14"/>
       <c r="N11" s="14"/>
       <c r="O11"/>
       <c r="Q11" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="2:18" ht="119">
       <c r="B12" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="C12" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="G12" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J12" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="L12" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="I12" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>69</v>
-      </c>
       <c r="M12" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O12"/>
       <c r="Q12" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R12" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="255">
+      <c r="C13" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="24" t="s">
+        <v>159</v>
+      </c>
+      <c r="G13" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J13" s="38" t="s">
+        <v>157</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N13" s="2" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" ht="221">
-      <c r="C13" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="O13"/>
       <c r="Q13" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" ht="153">
-      <c r="C14" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" ht="221">
+      <c r="C14" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="35"/>
+      <c r="F14" s="24" t="s">
+        <v>158</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="O14"/>
+      <c r="Q14" s="7"/>
+    </row>
+    <row r="15" spans="2:18" ht="153">
+      <c r="C15" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="M15" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="O15"/>
+      <c r="Q15" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="R15" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" s="8" customFormat="1">
+      <c r="C16" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J14" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="N14" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="O14"/>
-      <c r="Q14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="R14" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" spans="2:18" s="8" customFormat="1">
-      <c r="C15" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="F16" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="14"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
-    </row>
-    <row r="16" spans="2:18">
-      <c r="B16" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
+      <c r="G16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="L16" s="2"/>
+      <c r="M16" s="2"/>
+      <c r="N16" s="14"/>
       <c r="O16"/>
       <c r="P16"/>
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="2:18" ht="153">
-      <c r="C17" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="5" t="s">
+    <row r="17" spans="2:18">
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="29" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F17" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J17" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M17" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>104</v>
-      </c>
+      <c r="F17" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="J17" s="37" t="s">
+        <v>60</v>
+      </c>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
       <c r="O17"/>
       <c r="P17"/>
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="2:18">
+    <row r="18" spans="2:18" ht="153">
       <c r="C18" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>48</v>
+        <v>34</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>8</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="I18" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="2" t="s">
-        <v>91</v>
+        <v>44</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M18" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="O18"/>
       <c r="P18"/>
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="2:18" ht="136">
+    <row r="19" spans="2:18">
       <c r="C19" s="7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G19" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J19" s="11" t="s">
-        <v>128</v>
+        <v>12</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="L19" s="14"/>
-      <c r="M19" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="N19" s="14" t="s">
-        <v>105</v>
+      <c r="M19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="O19"/>
       <c r="P19"/>
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="2:18" ht="221">
+    <row r="20" spans="2:18" ht="136">
       <c r="C20" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G20" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="L20" s="14"/>
+      <c r="M20" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="N20" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+    </row>
+    <row r="21" spans="2:18" ht="221">
+      <c r="C21" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="L21" s="14"/>
+      <c r="M21" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="N21" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" s="8" customFormat="1" ht="153">
+      <c r="C22" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="J20" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="N20" s="11" t="s">
+      <c r="D22" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J22" s="12" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="21" spans="2:18" s="8" customFormat="1" ht="153">
-      <c r="C21" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G21" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="H21" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J21" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="L21" s="2"/>
-      <c r="M21" s="14"/>
-      <c r="N21" s="14"/>
-    </row>
-    <row r="22" spans="2:18">
-      <c r="C22" s="7"/>
+      <c r="L22" s="2"/>
       <c r="M22" s="14"/>
       <c r="N22" s="14"/>
     </row>
-    <row r="23" spans="2:18" s="8" customFormat="1" ht="187">
-      <c r="B23" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D23" s="8" t="s">
+    <row r="23" spans="2:18">
+      <c r="C23" s="7"/>
+      <c r="M23" s="14"/>
+      <c r="N23" s="14"/>
+    </row>
+    <row r="24" spans="2:18" s="8" customFormat="1" ht="187">
+      <c r="B24" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E23" s="10" t="s">
+      <c r="E24" s="10" t="s">
         <v>6</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G23" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="H23" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J23" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" s="8" customFormat="1" ht="187">
-      <c r="C24" s="9"/>
-      <c r="D24" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>55</v>
       </c>
       <c r="F24" s="8" t="s">
         <v>22</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H24" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I24" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" s="8" customFormat="1" ht="187">
+      <c r="C25" s="9"/>
+      <c r="D25" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="H25" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="J24" s="12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" s="8" customFormat="1" ht="221">
-      <c r="C25" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="D25" s="8" t="s">
+      <c r="I25" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" s="8" customFormat="1" ht="221">
+      <c r="C26" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="H25" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="J25" s="12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" s="8" customFormat="1" ht="153">
-      <c r="C26" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>91</v>
+      <c r="G26" s="12" t="s">
+        <v>98</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="J26" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="2:18" s="8" customFormat="1" ht="221">
+    <row r="27" spans="2:18" s="8" customFormat="1" ht="153">
       <c r="C27" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>53</v>
+        <v>22</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H27" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I27" s="8" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="J27" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="L27" s="14"/>
-      <c r="M27" s="14"/>
-      <c r="N27" s="14"/>
-      <c r="O27" s="14"/>
-    </row>
-    <row r="28" spans="2:18" s="8" customFormat="1" ht="119">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" s="8" customFormat="1" ht="221">
       <c r="C28" s="9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+      <c r="N28" s="14"/>
+      <c r="O28" s="14"/>
+    </row>
+    <row r="29" spans="2:18" s="8" customFormat="1" ht="119">
+      <c r="C29" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H28" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J28" s="12" t="s">
-        <v>118</v>
+      <c r="G29" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2625,10 +2746,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD210C5-361F-8048-B73A-B4DC7D734145}">
-  <dimension ref="B1:M31"/>
+  <dimension ref="B1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2637,20 +2758,20 @@
     <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="29" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" customWidth="1"/>
     <col min="11" max="12" width="15.6640625" customWidth="1"/>
     <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13">
       <c r="F1" s="23" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="2:13">
       <c r="B2" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="22"/>
@@ -2664,131 +2785,131 @@
         <v>4</v>
       </c>
       <c r="C3" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="D3" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="D3" s="17" t="s">
-        <v>75</v>
-      </c>
       <c r="K3" s="17" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="L3" s="17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="2:13">
       <c r="B4" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>104</v>
+        <v>58</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>103</v>
       </c>
       <c r="E4" s="18"/>
-      <c r="K4" s="26" t="s">
-        <v>138</v>
-      </c>
-      <c r="L4" s="26" t="s">
-        <v>139</v>
+      <c r="K4" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="L4" s="24" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="2"/>
-      <c r="C5" s="16" t="s">
-        <v>81</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>76</v>
+      <c r="C5" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="E5" s="18"/>
     </row>
     <row r="6" spans="2:13">
       <c r="B6" s="2"/>
-      <c r="C6" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>106</v>
+      <c r="C6" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="E6" s="18"/>
     </row>
     <row r="7" spans="2:13">
       <c r="B7" s="2"/>
-      <c r="C7" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>107</v>
+      <c r="C7" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" s="24" t="s">
+        <v>75</v>
       </c>
       <c r="E7" s="18"/>
       <c r="K7" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="L7" s="17" t="s">
         <v>134</v>
-      </c>
-      <c r="L7" s="17" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="2"/>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="21" t="s">
-        <v>93</v>
-      </c>
       <c r="E8" s="18"/>
-      <c r="K8" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="L8" t="s">
-        <v>139</v>
+      <c r="K8" s="25" t="s">
+        <v>138</v>
+      </c>
+      <c r="L8" s="25" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="2"/>
-      <c r="C9" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>101</v>
+      <c r="C9" s="31" t="s">
+        <v>102</v>
+      </c>
+      <c r="D9" s="31" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="2:13" ht="17">
       <c r="B10" s="2"/>
-      <c r="C10" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>101</v>
+      <c r="C10" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" s="33" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="11" spans="2:13" ht="17">
       <c r="B11" s="2"/>
       <c r="C11" s="14"/>
-      <c r="D11" s="25" t="s">
-        <v>109</v>
+      <c r="D11" s="33" t="s">
+        <v>108</v>
       </c>
       <c r="K11" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="L11" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="L11" s="17" t="s">
-        <v>137</v>
-      </c>
       <c r="M11" s="17" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="12" spans="2:13" s="23" customFormat="1">
-      <c r="K12" s="29" t="s">
+      <c r="K12" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="L12" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="M12" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="L12" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="M12" s="23" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="13" spans="2:13" s="23" customFormat="1">
@@ -2796,209 +2917,249 @@
         <v>4</v>
       </c>
       <c r="G13" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="H13" s="17" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="14" spans="2:13" s="23" customFormat="1">
       <c r="B14" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C14" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D14" s="14"/>
       <c r="F14" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>104</v>
+        <v>71</v>
+      </c>
+      <c r="G14" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="2:13" s="23" customFormat="1">
-      <c r="C15" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D15" s="14"/>
+      <c r="C15" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D15" s="26"/>
       <c r="F15" s="16"/>
-      <c r="G15" s="19" t="s">
+      <c r="G15" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K15" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="L15" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="M15" s="17" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" s="23" customFormat="1" ht="17">
+      <c r="C16" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="M16" s="23" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="23" customFormat="1" ht="17">
+      <c r="C17" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D17" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="16"/>
+      <c r="G17" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K15" s="17" t="s">
-        <v>136</v>
-      </c>
-      <c r="L15" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="M15" s="17" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13" s="23" customFormat="1" ht="17">
-      <c r="C16" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F16" s="16"/>
-      <c r="G16" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="K16" s="23" t="s">
-        <v>141</v>
-      </c>
-      <c r="L16" s="29" t="s">
-        <v>141</v>
-      </c>
-      <c r="M16" s="23" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" s="23" customFormat="1" ht="17">
-      <c r="C17" s="30" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>76</v>
+      <c r="H17" s="24" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="18" spans="2:8" s="23" customFormat="1">
       <c r="F18" s="16"/>
-      <c r="G18" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>108</v>
+      <c r="G18" s="29" t="s">
+        <v>145</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="2:8" s="23" customFormat="1">
       <c r="E19" s="14"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="7" t="s">
+      <c r="F19" s="16"/>
+      <c r="G19" s="29" t="s">
+        <v>146</v>
+      </c>
+      <c r="H19" s="24" t="s">
         <v>75</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="20" spans="2:8" s="23" customFormat="1">
       <c r="B20" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>104</v>
+        <v>70</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="26" t="s">
+        <v>103</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>100</v>
+      <c r="G20" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="2:8" s="23" customFormat="1">
       <c r="B21" s="14"/>
-      <c r="C21" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>146</v>
+      <c r="C21" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>144</v>
       </c>
       <c r="F21" s="2"/>
-      <c r="G21" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" s="23" customFormat="1">
+      <c r="G21" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="24" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" s="23" customFormat="1" ht="17">
       <c r="B22" s="14"/>
-      <c r="C22" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D22" s="14" t="s">
-        <v>101</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="24" t="s">
-        <v>89</v>
-      </c>
-      <c r="H22" s="14" t="s">
-        <v>100</v>
+      <c r="C22" s="27" t="s">
+        <v>160</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" s="2"/>
+      <c r="G22" s="29" t="s">
+        <v>150</v>
+      </c>
+      <c r="H22" s="24" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="2:8" s="23" customFormat="1">
       <c r="F23" s="14"/>
-      <c r="G23" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>100</v>
+      <c r="G23" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="H23" s="26" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="2:8" s="23" customFormat="1">
       <c r="F24" s="14"/>
-      <c r="G24" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" s="23" customFormat="1"/>
+      <c r="G24" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="H24" s="26" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" s="23" customFormat="1">
+      <c r="F25" s="14"/>
+      <c r="G25" s="31" t="s">
+        <v>95</v>
+      </c>
+      <c r="H25" s="31" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="26" spans="2:8" s="23" customFormat="1"/>
     <row r="27" spans="2:8" s="23" customFormat="1"/>
-    <row r="28" spans="2:8" s="23" customFormat="1">
-      <c r="F28" s="23" t="s">
-        <v>130</v>
-      </c>
-    </row>
+    <row r="28" spans="2:8" s="23" customFormat="1"/>
     <row r="29" spans="2:8" s="23" customFormat="1">
-      <c r="F29" s="14"/>
-      <c r="G29" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="H29" s="14"/>
-    </row>
-    <row r="30" spans="2:8" ht="17">
-      <c r="F30" s="23"/>
-      <c r="G30" s="30" t="s">
-        <v>131</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>101</v>
-      </c>
+      <c r="F29" s="23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="F30" s="14"/>
+      <c r="G30" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H30" s="31"/>
     </row>
     <row r="31" spans="2:8" ht="17">
       <c r="F31" s="23"/>
-      <c r="G31" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="H31" s="31" t="s">
-        <v>101</v>
+      <c r="G31" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="H31" s="28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" ht="17">
+      <c r="F32" s="23"/>
+      <c r="G32" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" s="28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="6:8">
+      <c r="F34" s="20" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+    </row>
+    <row r="35" spans="6:8">
+      <c r="F35" s="14"/>
+      <c r="G35" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="H35" s="31"/>
+    </row>
+    <row r="36" spans="6:8" ht="17">
+      <c r="F36" s="23"/>
+      <c r="G36" s="27" t="s">
+        <v>163</v>
+      </c>
+      <c r="H36" s="28" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="37" spans="6:8" ht="17">
+      <c r="F37" s="23"/>
+      <c r="G37" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="H37" s="28" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All models and routes working previous to passport authentication
</commit_message>
<xml_diff>
--- a/books-apis-baseline.xlsx
+++ b/books-apis-baseline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorge_guzman/bootCampClasses/projects/project2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC21A9-B795-D341-879D-53481EEA5E0D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73A7F30-8BE1-FC40-8D6A-69570572015A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25100" windowHeight="22660" activeTab="1" xr2:uid="{86F54AEE-F7BE-1B46-B9C2-50DD7E0F702B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="171">
   <si>
     <t>Sign up / Log in</t>
   </si>
@@ -687,6 +687,9 @@
         "Shoppingcart": null,
         "Purchases": []
     }</t>
+  </si>
+  <si>
+    <t>shoppingcarts-books</t>
   </si>
 </sst>
 </file>
@@ -818,7 +821,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -874,8 +877,8 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -954,6 +957,7 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1935,7 +1939,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2946,7 +2950,7 @@
   <dimension ref="B1:L39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3119,10 +3123,10 @@
       </c>
     </row>
     <row r="14" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="J14" s="16" t="s">
+      <c r="J14" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="K14" s="16" t="s">
+      <c r="K14" s="49" t="s">
         <v>137</v>
       </c>
       <c r="L14" s="11" t="s">
@@ -3193,10 +3197,10 @@
       <c r="H18" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="J18" s="16" t="s">
+      <c r="J18" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="K18" s="16" t="s">
+      <c r="K18" s="49" t="s">
         <v>137</v>
       </c>
       <c r="L18" s="11" t="s">
@@ -3318,22 +3322,22 @@
     <row r="29" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="30" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F30" s="9" t="s">
-        <v>141</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="2:12" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="F31" s="5"/>
-      <c r="G31" s="21" t="s">
+      <c r="G31" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="H31" s="21"/>
+      <c r="H31" s="15"/>
     </row>
     <row r="32" spans="2:12" ht="17" x14ac:dyDescent="0.2">
       <c r="F32" s="11"/>
       <c r="G32" s="16" t="s">
         <v>161</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="21" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3342,7 +3346,7 @@
       <c r="G33" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="21" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3355,17 +3359,17 @@
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F37" s="5"/>
-      <c r="G37" s="21" t="s">
+      <c r="G37" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="H37" s="21"/>
+      <c r="H37" s="15"/>
     </row>
     <row r="38" spans="6:8" ht="17" x14ac:dyDescent="0.2">
       <c r="F38" s="11"/>
       <c r="G38" s="16" t="s">
         <v>160</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="21" t="s">
         <v>152</v>
       </c>
     </row>
@@ -3374,7 +3378,7 @@
       <c r="G39" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H39" s="21" t="s">
         <v>152</v>
       </c>
     </row>

</xml_diff>